<commit_message>
NASS and CRP nr inflation adjustments; substitute 2008NASS data for 2007NASS data because more resolution; make county panel random sample
</commit_message>
<xml_diff>
--- a/results/initial_descriptives/combined/countypanel_variables.xlsx
+++ b/results/initial_descriptives/combined/countypanel_variables.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="162">
   <si>
     <t>position</t>
   </si>
@@ -345,9 +345,6 @@
     <t>state+county fips code</t>
   </si>
   <si>
-    <t>YEAR</t>
-  </si>
-  <si>
     <t>(sum) acresk</t>
   </si>
   <si>
@@ -402,7 +399,7 @@
     <t>obs has NRI(6classes), CRP, and 4 NR data components</t>
   </si>
   <si>
-    <t>RENT, CASH, PASTURELAND - EXPENSE, MEASURED IN $ / ACRE</t>
+    <t>2010USD pastureland rent/acre (NASS)</t>
   </si>
   <si>
     <t>Pasture rents (NASS) data level</t>
@@ -411,10 +408,10 @@
     <t>Thousand acres in CRP (USDA County Stats)</t>
   </si>
   <si>
-    <t>CRP Contract-based FY rental payments (not actuals) (USDA County Stats)</t>
-  </si>
-  <si>
-    <t>avg per-CRPacre contract-based FY rent payments (not actuals) (USDA County Stats</t>
+    <t>2010USD CRP Contract-based FY rent payments (not actuals) (USDA)</t>
+  </si>
+  <si>
+    <t>2010USD avg per-CRPacre contract-based FY rent payments (not actuals) (USDA)</t>
   </si>
   <si>
     <t>2010USD annualized net return/acre net income deriving from crop production[L&amp;M]</t>
@@ -683,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -700,7 +697,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10">
@@ -717,7 +714,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11">
@@ -734,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12">
@@ -751,7 +748,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13">
@@ -768,7 +765,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14">
@@ -785,7 +782,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15">
@@ -802,7 +799,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16">
@@ -819,7 +816,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17">
@@ -836,7 +833,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18">
@@ -853,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19">
@@ -870,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20">
@@ -887,7 +884,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21">
@@ -904,7 +901,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22">
@@ -921,7 +918,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23">
@@ -938,7 +935,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24">
@@ -955,7 +952,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25">
@@ -972,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26">
@@ -989,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27">
@@ -1006,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28">
@@ -1023,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29">
@@ -1040,7 +1037,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30">
@@ -1057,7 +1054,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31">
@@ -1074,7 +1071,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32">
@@ -1091,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33">
@@ -1108,7 +1105,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34">
@@ -1125,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35">
@@ -1142,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36">
@@ -1159,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37">
@@ -1176,7 +1173,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38">
@@ -1193,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39">
@@ -1210,7 +1207,7 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40">
@@ -1227,7 +1224,7 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41">
@@ -1244,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42">
@@ -1261,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43">
@@ -1278,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44">
@@ -1295,7 +1292,7 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45">
@@ -1312,7 +1309,7 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46">
@@ -1329,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47">
@@ -1346,7 +1343,7 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48">
@@ -1363,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49">
@@ -1380,7 +1377,7 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50">
@@ -1397,7 +1394,7 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51">
@@ -1414,7 +1411,7 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52">
@@ -1431,7 +1428,7 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53">
@@ -1448,7 +1445,7 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54">
@@ -1465,7 +1462,7 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55">
@@ -1482,7 +1479,7 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56">
@@ -1499,7 +1496,7 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57">
@@ -1516,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58">
@@ -1533,7 +1530,7 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59">
@@ -1550,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60">
@@ -1567,7 +1564,7 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61">
@@ -1584,7 +1581,7 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62">
@@ -1601,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63">
@@ -1618,7 +1615,7 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64">
@@ -1635,7 +1632,7 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="65">
@@ -1652,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="66">
@@ -1669,7 +1666,7 @@
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67">
@@ -1686,7 +1683,7 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68">
@@ -1703,7 +1700,7 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="69">
@@ -1720,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="70">
@@ -1737,7 +1734,7 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="71">
@@ -1754,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="72">
@@ -1771,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="73">
@@ -1788,7 +1785,7 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="74">
@@ -1805,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="75">
@@ -1822,7 +1819,7 @@
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="76">
@@ -1839,7 +1836,7 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="77">
@@ -1856,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="78">
@@ -1873,7 +1870,7 @@
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79">
@@ -1890,7 +1887,7 @@
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="80">
@@ -1907,7 +1904,7 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81">
@@ -1924,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="82">
@@ -1941,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="83">
@@ -1958,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="84">
@@ -1975,7 +1972,7 @@
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85">
@@ -1992,7 +1989,7 @@
         <v>0</v>
       </c>
       <c r="E85" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86">
@@ -2009,7 +2006,7 @@
         <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="87">
@@ -2026,7 +2023,7 @@
         <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
incorporate new urban net returns data 1
</commit_message>
<xml_diff>
--- a/results/initial_descriptives/combined/countypanel_variables.xlsx
+++ b/results/initial_descriptives/combined/countypanel_variables.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="160">
   <si>
     <t>position</t>
   </si>
@@ -39,6 +39,9 @@
     <t>fips</t>
   </si>
   <si>
+    <t>fipsstr</t>
+  </si>
+  <si>
     <t>year</t>
   </si>
   <si>
@@ -294,6 +297,9 @@
     <t>long</t>
   </si>
   <si>
+    <t>str5</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
@@ -330,6 +336,9 @@
     <t>state+county fips code</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>(sum) acresk</t>
   </si>
   <si>
@@ -396,7 +405,7 @@
     <t>2010USD annualized net return/acre of bare forestland [L&amp;M]</t>
   </si>
   <si>
-    <t>2010USD annualized net return/acre derived from price of recently dev. land[L&amp;M]</t>
+    <t>2010USD annualized net return/acre [RFF]</t>
   </si>
   <si>
     <t>= pasture_nr</t>
@@ -529,7 +538,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E86"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -540,13 +549,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2">
@@ -557,13 +566,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3">
@@ -574,13 +583,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4">
@@ -591,13 +600,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5">
@@ -608,13 +617,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6">
@@ -625,13 +634,13 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7">
@@ -642,13 +651,13 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8">
@@ -659,13 +668,13 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9">
@@ -676,13 +685,13 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
@@ -693,13 +702,13 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11">
@@ -710,13 +719,13 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12">
@@ -727,13 +736,13 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
@@ -744,13 +753,13 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14">
@@ -761,13 +770,13 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15">
@@ -778,13 +787,13 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16">
@@ -795,13 +804,13 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17">
@@ -812,13 +821,13 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18">
@@ -829,13 +838,13 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19">
@@ -846,13 +855,13 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20">
@@ -863,13 +872,13 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21">
@@ -880,13 +889,13 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22">
@@ -897,13 +906,13 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23">
@@ -914,13 +923,13 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24">
@@ -931,13 +940,13 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25">
@@ -948,13 +957,13 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26">
@@ -965,13 +974,13 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27">
@@ -982,13 +991,13 @@
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28">
@@ -999,13 +1008,13 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29">
@@ -1016,13 +1025,13 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30">
@@ -1033,13 +1042,13 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31">
@@ -1050,13 +1059,13 @@
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32">
@@ -1067,13 +1076,13 @@
         <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33">
@@ -1084,13 +1093,13 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34">
@@ -1101,13 +1110,13 @@
         <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35">
@@ -1118,13 +1127,13 @@
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36">
@@ -1135,13 +1144,13 @@
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37">
@@ -1152,13 +1161,13 @@
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D37" s="1">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38">
@@ -1169,13 +1178,13 @@
         <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39">
@@ -1186,13 +1195,13 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D39" s="1">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40">
@@ -1203,13 +1212,13 @@
         <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41">
@@ -1220,13 +1229,13 @@
         <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42">
@@ -1237,13 +1246,13 @@
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43">
@@ -1254,13 +1263,13 @@
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44">
@@ -1271,13 +1280,13 @@
         <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45">
@@ -1288,13 +1297,13 @@
         <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46">
@@ -1305,13 +1314,13 @@
         <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47">
@@ -1322,13 +1331,13 @@
         <v>47</v>
       </c>
       <c r="C47" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48">
@@ -1339,13 +1348,13 @@
         <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49">
@@ -1356,13 +1365,13 @@
         <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50">
@@ -1373,13 +1382,13 @@
         <v>50</v>
       </c>
       <c r="C50" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D50" s="1">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51">
@@ -1390,13 +1399,13 @@
         <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D51" s="1">
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52">
@@ -1407,13 +1416,13 @@
         <v>52</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D52" s="1">
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53">
@@ -1424,13 +1433,13 @@
         <v>53</v>
       </c>
       <c r="C53" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D53" s="1">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54">
@@ -1441,13 +1450,13 @@
         <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D54" s="1">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55">
@@ -1458,13 +1467,13 @@
         <v>55</v>
       </c>
       <c r="C55" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D55" s="1">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56">
@@ -1475,13 +1484,13 @@
         <v>56</v>
       </c>
       <c r="C56" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D56" s="1">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57">
@@ -1492,13 +1501,13 @@
         <v>57</v>
       </c>
       <c r="C57" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58">
@@ -1509,13 +1518,13 @@
         <v>58</v>
       </c>
       <c r="C58" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D58" s="1">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59">
@@ -1526,13 +1535,13 @@
         <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D59" s="1">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60">
@@ -1543,13 +1552,13 @@
         <v>60</v>
       </c>
       <c r="C60" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D60" s="1">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61">
@@ -1560,13 +1569,13 @@
         <v>61</v>
       </c>
       <c r="C61" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D61" s="1">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62">
@@ -1577,13 +1586,13 @@
         <v>62</v>
       </c>
       <c r="C62" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D62" s="1">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63">
@@ -1594,13 +1603,13 @@
         <v>63</v>
       </c>
       <c r="C63" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D63" s="1">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64">
@@ -1611,13 +1620,13 @@
         <v>64</v>
       </c>
       <c r="C64" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D64" s="1">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65">
@@ -1628,13 +1637,13 @@
         <v>65</v>
       </c>
       <c r="C65" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D65" s="1">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66">
@@ -1645,13 +1654,13 @@
         <v>66</v>
       </c>
       <c r="C66" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D66" s="1">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67">
@@ -1662,13 +1671,13 @@
         <v>67</v>
       </c>
       <c r="C67" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D67" s="1">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="68">
@@ -1679,13 +1688,13 @@
         <v>68</v>
       </c>
       <c r="C68" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D68" s="1">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69">
@@ -1696,13 +1705,13 @@
         <v>69</v>
       </c>
       <c r="C69" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D69" s="1">
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="70">
@@ -1713,13 +1722,13 @@
         <v>70</v>
       </c>
       <c r="C70" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D70" s="1">
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71">
@@ -1730,13 +1739,13 @@
         <v>71</v>
       </c>
       <c r="C71" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D71" s="1">
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="72">
@@ -1747,13 +1756,13 @@
         <v>72</v>
       </c>
       <c r="C72" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D72" s="1">
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73">
@@ -1764,13 +1773,13 @@
         <v>73</v>
       </c>
       <c r="C73" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D73" s="1">
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="74">
@@ -1781,13 +1790,13 @@
         <v>74</v>
       </c>
       <c r="C74" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D74" s="1">
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75">
@@ -1798,13 +1807,13 @@
         <v>75</v>
       </c>
       <c r="C75" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D75" s="1">
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76">
@@ -1815,13 +1824,13 @@
         <v>76</v>
       </c>
       <c r="C76" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D76" s="1">
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="77">
@@ -1832,13 +1841,13 @@
         <v>77</v>
       </c>
       <c r="C77" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D77" s="1">
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78">
@@ -1849,13 +1858,13 @@
         <v>78</v>
       </c>
       <c r="C78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D78" s="1">
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="79">
@@ -1866,13 +1875,13 @@
         <v>79</v>
       </c>
       <c r="C79" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D79" s="1">
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80">
@@ -1883,13 +1892,13 @@
         <v>80</v>
       </c>
       <c r="C80" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D80" s="1">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81">
@@ -1900,13 +1909,13 @@
         <v>81</v>
       </c>
       <c r="C81" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D81" s="1">
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82">
@@ -1917,13 +1926,13 @@
         <v>82</v>
       </c>
       <c r="C82" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D82" s="1">
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83">
@@ -1934,13 +1943,13 @@
         <v>83</v>
       </c>
       <c r="C83" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D83" s="1">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84">
@@ -1951,13 +1960,13 @@
         <v>84</v>
       </c>
       <c r="C84" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D84" s="1">
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85">
@@ -1968,13 +1977,30 @@
         <v>85</v>
       </c>
       <c r="C85" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D85" s="1">
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>156</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>86</v>
+      </c>
+      <c r="C86" t="s">
+        <v>97</v>
+      </c>
+      <c r="D86" s="1">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>